<commit_message>
Minor update to code for combining all lists.
</commit_message>
<xml_diff>
--- a/data-raw/no-translation-now-translated.xlsx
+++ b/data-raw/no-translation-now-translated.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Primahadi/Documents/enggano-AHRC/enggano-holle-list-2023-03-27/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GRajeg\OneDrive - Nexus365\Documents\Research\barrier-island-Holle-list-2023-05-24\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FC89EF-D20A-C449-B0FF-CB1C950C5800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF225D84-9A2B-457F-8A77-404BA29F5B20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no-translation-now-translated" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="309">
   <si>
     <t>id</t>
   </si>
@@ -590,12 +577,6 @@
     <t>mimpi</t>
   </si>
   <si>
-    <t>its</t>
-  </si>
-  <si>
-    <t>-nya</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -830,12 +811,6 @@
     <t>ugly</t>
   </si>
   <si>
-    <t>fixed</t>
-  </si>
-  <si>
-    <t>tetap</t>
-  </si>
-  <si>
     <t>longgar</t>
   </si>
   <si>
@@ -966,6 +941,12 @@
   </si>
   <si>
     <t>rambut</t>
+  </si>
+  <si>
+    <t>terikat, kencang, erat</t>
+  </si>
+  <si>
+    <t>tightly bound, tightly fitting</t>
   </si>
 </sst>
 </file>
@@ -1809,16 +1790,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="163" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
   <cols>
     <col min="3" max="3" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1835,1061 +1814,1064 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.8">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>253</v>
+      </c>
+      <c r="E10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" t="s">
+        <v>258</v>
+      </c>
+      <c r="E11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D12" t="s">
+        <v>262</v>
+      </c>
+      <c r="E12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" t="s">
+        <v>264</v>
+      </c>
+      <c r="E14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D15" t="s">
+        <v>305</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>305</v>
+      </c>
+      <c r="E16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" t="s">
+        <v>267</v>
+      </c>
+      <c r="E18" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" t="s">
+        <v>269</v>
+      </c>
+      <c r="E19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>271</v>
+      </c>
+      <c r="E20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" t="s">
+        <v>273</v>
+      </c>
+      <c r="E21" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" t="s">
+        <v>275</v>
+      </c>
+      <c r="E22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" t="s">
+        <v>277</v>
+      </c>
+      <c r="E23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" t="s">
+        <v>279</v>
+      </c>
+      <c r="E24" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" t="s">
+        <v>281</v>
+      </c>
+      <c r="E25" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>283</v>
+      </c>
+      <c r="E26" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" t="s">
+        <v>285</v>
+      </c>
+      <c r="E27" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" t="s">
+        <v>287</v>
+      </c>
+      <c r="E28" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" t="s">
+        <v>289</v>
+      </c>
+      <c r="E29" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" t="s">
+        <v>291</v>
+      </c>
+      <c r="E30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" t="s">
+        <v>293</v>
+      </c>
+      <c r="E31" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" t="s">
+        <v>295</v>
+      </c>
+      <c r="E32" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A34" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>297</v>
+      </c>
+      <c r="E34" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" t="s">
+        <v>299</v>
+      </c>
+      <c r="E35" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" t="s">
+        <v>301</v>
+      </c>
+      <c r="E36" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
         <v>185</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E37" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
         <v>187</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E38" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
         <v>189</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E39" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
         <v>191</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E40" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
         <v>193</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E41" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
         <v>195</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E42" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" t="s">
         <v>197</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E43" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" t="s">
         <v>199</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E44" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" t="s">
         <v>201</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E45" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" t="s">
         <v>203</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E46" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" t="s">
+        <v>206</v>
+      </c>
+      <c r="E47" t="s">
         <v>205</v>
       </c>
-      <c r="E13" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" t="s">
+        <v>303</v>
+      </c>
+      <c r="E48" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" t="s">
         <v>208</v>
       </c>
-      <c r="E14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
         <v>209</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E50" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" t="s">
         <v>211</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E51" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" t="s">
+        <v>214</v>
+      </c>
+      <c r="E52" t="s">
         <v>213</v>
       </c>
-      <c r="E17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" t="s">
+        <v>215</v>
+      </c>
+      <c r="E53" t="s">
         <v>216</v>
       </c>
-      <c r="E18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
         <v>217</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E54" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" t="s">
         <v>219</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E55" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" t="s">
         <v>221</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E56" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" t="s">
         <v>223</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E57" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" t="s">
         <v>225</v>
       </c>
-      <c r="E23" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" t="s">
+        <v>227</v>
+      </c>
+      <c r="E59" t="s">
         <v>228</v>
       </c>
-      <c r="E24" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" t="s">
         <v>229</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E60" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A61" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" t="s">
         <v>231</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E61" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A62" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" t="s">
         <v>233</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E62" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.8">
+      <c r="A63" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" t="s">
         <v>235</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E63" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>237</v>
-      </c>
-      <c r="E29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" t="s">
-        <v>239</v>
-      </c>
-      <c r="E30" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" t="s">
-        <v>241</v>
-      </c>
-      <c r="E31" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" t="s">
-        <v>242</v>
-      </c>
-      <c r="E32" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" t="s">
-        <v>254</v>
-      </c>
-      <c r="E33" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" t="s">
-        <v>244</v>
-      </c>
-      <c r="E34" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" t="s">
-        <v>245</v>
-      </c>
-      <c r="E35" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" t="s">
-        <v>246</v>
-      </c>
-      <c r="E36" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" t="s">
-        <v>247</v>
-      </c>
-      <c r="E37" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" t="s">
-        <v>255</v>
-      </c>
-      <c r="E38" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>257</v>
-      </c>
-      <c r="B39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" t="s">
-        <v>259</v>
-      </c>
-      <c r="D39" t="s">
-        <v>260</v>
-      </c>
-      <c r="E39" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>258</v>
-      </c>
-      <c r="B40" t="s">
-        <v>116</v>
-      </c>
-      <c r="C40" t="s">
-        <v>262</v>
-      </c>
-      <c r="D40" t="s">
-        <v>264</v>
-      </c>
-      <c r="E40" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41" t="s">
-        <v>265</v>
-      </c>
-      <c r="E41" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" t="s">
-        <v>268</v>
-      </c>
-      <c r="E42" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" t="s">
-        <v>269</v>
-      </c>
-      <c r="E43" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" t="s">
-        <v>128</v>
-      </c>
-      <c r="D44" t="s">
-        <v>271</v>
-      </c>
-      <c r="E44" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>129</v>
-      </c>
-      <c r="B45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" t="s">
-        <v>131</v>
-      </c>
-      <c r="D45" t="s">
-        <v>273</v>
-      </c>
-      <c r="E45" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" t="s">
-        <v>133</v>
-      </c>
-      <c r="C46" t="s">
-        <v>134</v>
-      </c>
-      <c r="D46" t="s">
-        <v>275</v>
-      </c>
-      <c r="E46" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" t="s">
-        <v>277</v>
-      </c>
-      <c r="E47" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>138</v>
-      </c>
-      <c r="B48" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" t="s">
-        <v>140</v>
-      </c>
-      <c r="D48" t="s">
-        <v>279</v>
-      </c>
-      <c r="E48" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" t="s">
-        <v>143</v>
-      </c>
-      <c r="D49" t="s">
-        <v>281</v>
-      </c>
-      <c r="E49" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" t="s">
-        <v>145</v>
-      </c>
-      <c r="C50" t="s">
-        <v>146</v>
-      </c>
-      <c r="D50" t="s">
-        <v>283</v>
-      </c>
-      <c r="E50" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>147</v>
-      </c>
-      <c r="B51" t="s">
-        <v>148</v>
-      </c>
-      <c r="C51" t="s">
-        <v>149</v>
-      </c>
-      <c r="D51" t="s">
-        <v>285</v>
-      </c>
-      <c r="E51" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>150</v>
-      </c>
-      <c r="B52" t="s">
-        <v>151</v>
-      </c>
-      <c r="C52" t="s">
-        <v>152</v>
-      </c>
-      <c r="D52" t="s">
-        <v>287</v>
-      </c>
-      <c r="E52" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>153</v>
-      </c>
-      <c r="B53" t="s">
-        <v>154</v>
-      </c>
-      <c r="C53" t="s">
-        <v>155</v>
-      </c>
-      <c r="D53" t="s">
-        <v>289</v>
-      </c>
-      <c r="E53" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>156</v>
-      </c>
-      <c r="B54" t="s">
-        <v>157</v>
-      </c>
-      <c r="C54" t="s">
-        <v>158</v>
-      </c>
-      <c r="D54" t="s">
-        <v>291</v>
-      </c>
-      <c r="E54" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C55" t="s">
-        <v>161</v>
-      </c>
-      <c r="D55" t="s">
-        <v>293</v>
-      </c>
-      <c r="E55" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>162</v>
-      </c>
-      <c r="B56" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" t="s">
-        <v>164</v>
-      </c>
-      <c r="D56" t="s">
-        <v>295</v>
-      </c>
-      <c r="E56" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>165</v>
-      </c>
-      <c r="B57" t="s">
-        <v>163</v>
-      </c>
-      <c r="C57" t="s">
-        <v>166</v>
-      </c>
-      <c r="D57" t="s">
-        <v>297</v>
-      </c>
-      <c r="E57" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>167</v>
-      </c>
-      <c r="B58" t="s">
-        <v>168</v>
-      </c>
-      <c r="C58" t="s">
-        <v>169</v>
-      </c>
-      <c r="D58" t="s">
-        <v>299</v>
-      </c>
-      <c r="E58" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>170</v>
-      </c>
-      <c r="B59" t="s">
-        <v>171</v>
-      </c>
-      <c r="C59" t="s">
-        <v>172</v>
-      </c>
-      <c r="D59" t="s">
-        <v>301</v>
-      </c>
-      <c r="E59" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>173</v>
-      </c>
-      <c r="B60" t="s">
-        <v>174</v>
-      </c>
-      <c r="C60" t="s">
-        <v>175</v>
-      </c>
-      <c r="D60" t="s">
-        <v>303</v>
-      </c>
-      <c r="E60" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>176</v>
-      </c>
-      <c r="B61" t="s">
-        <v>177</v>
-      </c>
-      <c r="C61" t="s">
-        <v>178</v>
-      </c>
-      <c r="D61" t="s">
-        <v>305</v>
-      </c>
-      <c r="E61" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>179</v>
-      </c>
-      <c r="B62" t="s">
-        <v>180</v>
-      </c>
-      <c r="C62" t="s">
-        <v>181</v>
-      </c>
-      <c r="D62" t="s">
-        <v>307</v>
-      </c>
-      <c r="E62" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" t="s">
-        <v>182</v>
-      </c>
-      <c r="C63" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" t="s">
-        <v>309</v>
-      </c>
-      <c r="E63" t="s">
-        <v>310</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:E63">
+    <sortCondition ref="A2:A63"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>